<commit_message>
V2: se agregó control para fechas, archivos, id de peticiones, %
</commit_message>
<xml_diff>
--- a/POA2018.xlsx
+++ b/POA2018.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="83">
   <si>
     <t>Desarrollo</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Apoyo al departamento de Comunicaciones en la integración al Portal Único del Estado</t>
   </si>
   <si>
-    <t>Creación y mantenimiento de una base de datos de gestión de configuración (CMDB)</t>
-  </si>
-  <si>
     <t>Implantación de un sistema integral de seguridad informática</t>
   </si>
   <si>
@@ -271,13 +268,19 @@
   </si>
   <si>
     <t>Tareas</t>
+  </si>
+  <si>
+    <t>Incorporar el rol de sustentabilidad de trámites</t>
+  </si>
+  <si>
+    <t>Fecha de inicio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +298,13 @@
     <font>
       <sz val="10"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF484848"/>
+      <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -318,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -327,6 +337,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,7 +622,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,31 +632,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4">
-        <v>81</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -655,40 +667,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
     <col min="3" max="3" width="44.85546875" customWidth="1"/>
     <col min="4" max="4" width="61.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -702,13 +718,16 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G2" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -716,19 +735,22 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G3" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -736,19 +758,22 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G4" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -756,19 +781,22 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G5" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -776,19 +804,22 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G6" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -796,19 +827,22 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G7" s="5">
+        <v>43103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -816,19 +850,22 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G8" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -836,19 +873,22 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G9" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -856,19 +896,22 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G10" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -876,19 +919,22 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G11" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -896,19 +942,22 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G12" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -916,19 +965,22 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G13" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -936,119 +988,137 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="E14" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>35</v>
       </c>
-      <c r="E15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>36</v>
       </c>
-      <c r="E16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
         <v>37</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>37</v>
       </c>
-      <c r="E17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
         <v>38</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>38</v>
       </c>
-      <c r="E18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G19" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1056,19 +1126,22 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G20" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1076,19 +1149,22 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G21" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1096,19 +1172,22 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G22" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1116,19 +1195,22 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G23" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1136,19 +1218,22 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G24" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1156,19 +1241,22 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G25" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1176,19 +1264,22 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G26" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1196,19 +1287,22 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G27" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1216,19 +1310,22 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G28" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1236,279 +1333,321 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G29" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G30" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G31" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G32" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G33" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G34" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G35" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G36" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F37" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G37" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F38" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G38" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F39" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G39" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F40" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G40" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F41" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G41" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G42" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1516,19 +1655,22 @@
         <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="D43" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="E43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F43" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G43" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1536,19 +1678,22 @@
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D44" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G44" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -1556,19 +1701,22 @@
         <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D45" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F45" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G45" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -1576,19 +1724,22 @@
         <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="E46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F46" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G46" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -1602,173 +1753,200 @@
         <v>11</v>
       </c>
       <c r="E47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F47" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G47" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F48" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G48" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F49" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G49" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F50" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G50" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F51" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G51" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F52" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G52" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F53" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G53" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F54" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G54" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F55" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G55" s="5">
+        <v>43102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1776,56 +1954,19 @@
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F56" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" t="s">
-        <v>13</v>
-      </c>
-      <c r="E57" t="s">
-        <v>66</v>
-      </c>
-      <c r="F57" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" t="s">
-        <v>14</v>
-      </c>
-      <c r="E58" t="s">
-        <v>66</v>
-      </c>
-      <c r="F58" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="G56" s="5">
+        <v>43102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V3: se agregó la configuración de los campos como parámetros y se incorporó la opciòn de Modo de operación para cargar o sólo validar
</commit_message>
<xml_diff>
--- a/POA2018.xlsx
+++ b/POA2018.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="84">
   <si>
     <t>Desarrollo</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Fecha de inicio</t>
+  </si>
+  <si>
+    <t>dddd</t>
   </si>
 </sst>
 </file>
@@ -667,10 +670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:K1048576"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +684,7 @@
     <col min="4" max="4" width="61.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -703,8 +706,11 @@
       <c r="G1" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -727,7 +733,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -750,7 +756,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -773,7 +779,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -796,7 +802,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -819,7 +825,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -842,7 +848,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -865,7 +871,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -888,7 +894,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -911,7 +917,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -934,7 +940,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -957,7 +963,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -980,7 +986,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1009,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>43102</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>

</xml_diff>